<commit_message>
Module 2 Week 1 Example
</commit_message>
<xml_diff>
--- a/Module 2 Everyday Excel Part 2/Week 1 files/Comparing lists.xlsx
+++ b/Module 2 Everyday Excel Part 2/Week 1 files/Comparing lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\MOOC Excel\Screencasts\Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Week 1 files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8157E75-1CAE-4A6C-9B45-82AA8AC93D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53497ACF-FA8A-4FED-B27D-4CF8D054814C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{3178BD24-7150-4CEF-A6B8-3ABA03DDB18D}"/>
+    <workbookView xWindow="2145" yWindow="4545" windowWidth="28500" windowHeight="14955" xr2:uid="{3178BD24-7150-4CEF-A6B8-3ABA03DDB18D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,18 +18,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$2:$D$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -476,15 +468,15 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -504,57 +496,137 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C2" t="str">
+        <f>IF(COUNTIF($A$14:$A$19,A2),A2,"")</f>
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(COUNTIF($A$14:$A$19,A2),"",A2)</f>
+        <v>John</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C11" si="0">IF(COUNTIF($A$14:$A$19,A3),A3,"")</f>
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D11" si="1">IF(COUNTIF($A$14:$A$19,A3),"",A3)</f>
+        <v>Katie</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>Ella</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>Charlie</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>Max</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>Dana</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>Bob</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>Nancy</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Terry</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>Ezra</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -565,40 +637,88 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C14" t="str">
+        <f>IF(COUNTIF($A$2:$A$11,A14),A14,"")</f>
+        <v>Charlie</v>
+      </c>
+      <c r="D14" t="str">
+        <f>IF(COUNTIF($A$2:$A$11,A14),"",A14)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C15" t="str">
+        <f t="shared" ref="C15:C19" si="2">IF(COUNTIF($A$2:$A$11,A15),A15,"")</f>
+        <v>Terry</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" ref="D15:D19" si="3">IF(COUNTIF($A$2:$A$11,A15),"",A15)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C16" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="3"/>
+        <v>Jim</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C17" t="str">
+        <f t="shared" si="2"/>
+        <v>Ezra</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="3"/>
+        <v>Joe</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
+      <c r="C19" t="str">
+        <f t="shared" si="2"/>
+        <v>Max</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M20" t="s">
         <v>0</v>
       </c>

</xml_diff>